<commit_message>
Updated existing records - removed planned start and end dates and inserted 12 for the grant duration months following information from the Partnerships team. Amended the modified date for all records and added the URL to the Lab grant dataset webpage for the Data Source field.
</commit_message>
<xml_diff>
--- a/grants/trafford_council_voluntary_sector_grants_360_giving_format.xlsx
+++ b/grants/trafford_council_voluntary_sector_grants_360_giving_format.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Projects\360Giving\GrantNav_Files\20201111\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="grants" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2167" uniqueCount="618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2289" uniqueCount="619">
   <si>
     <t>Identifier</t>
   </si>
@@ -1873,6 +1878,9 @@
   </si>
   <si>
     <t>Trafford African &amp; caribbean over 50's club</t>
+  </si>
+  <si>
+    <t>https://www.trafforddatalab.io/open_data/grants/</t>
   </si>
 </sst>
 </file>
@@ -1911,13 +1919,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1927,6 +1936,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1975,7 +1987,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2010,7 +2022,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2219,21 +2231,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM123"/>
+  <dimension ref="A1:AM157"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AM1" sqref="AM1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="12" width="11.42578125"/>
-    <col min="13" max="13" width="46.7109375" customWidth="1"/>
-    <col min="14" max="14" width="57.28515625" customWidth="1"/>
-    <col min="15" max="15" width="28.140625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="30.28515625" style="1" customWidth="1"/>
-    <col min="17" max="1025" width="11.42578125"/>
+    <col min="1" max="12" width="11.453125"/>
+    <col min="13" max="13" width="46.7265625" customWidth="1"/>
+    <col min="14" max="14" width="57.26953125" customWidth="1"/>
+    <col min="15" max="15" width="28.1796875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="30.26953125" style="1" customWidth="1"/>
+    <col min="17" max="1025" width="11.453125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2352,7 +2366,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -2371,11 +2385,10 @@
       <c r="H2" s="2">
         <v>41292</v>
       </c>
-      <c r="J2" s="2">
-        <v>41000</v>
-      </c>
-      <c r="K2" s="2">
-        <v>41364</v>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="6">
+        <v>12</v>
       </c>
       <c r="M2" t="s">
         <v>522</v>
@@ -2417,10 +2430,13 @@
         <v>54</v>
       </c>
       <c r="AL2" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -2439,11 +2455,10 @@
       <c r="H3" s="2">
         <v>41292</v>
       </c>
-      <c r="J3" s="2">
-        <v>41000</v>
-      </c>
-      <c r="K3" s="2">
-        <v>41364</v>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="6">
+        <v>12</v>
       </c>
       <c r="M3" t="s">
         <v>523</v>
@@ -2490,10 +2505,13 @@
         <v>54</v>
       </c>
       <c r="AL3" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -2512,11 +2530,10 @@
       <c r="H4" s="2">
         <v>41292</v>
       </c>
-      <c r="J4" s="2">
-        <v>41000</v>
-      </c>
-      <c r="K4" s="2">
-        <v>41364</v>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="6">
+        <v>12</v>
       </c>
       <c r="M4" t="s">
         <v>524</v>
@@ -2563,10 +2580,13 @@
         <v>54</v>
       </c>
       <c r="AL4" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -2585,11 +2605,10 @@
       <c r="H5" s="2">
         <v>41292</v>
       </c>
-      <c r="J5" s="2">
-        <v>41000</v>
-      </c>
-      <c r="K5" s="2">
-        <v>41364</v>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="6">
+        <v>12</v>
       </c>
       <c r="M5" t="s">
         <v>525</v>
@@ -2642,10 +2661,13 @@
         <v>54</v>
       </c>
       <c r="AL5" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -2664,11 +2686,10 @@
       <c r="H6" s="2">
         <v>41292</v>
       </c>
-      <c r="J6" s="2">
-        <v>41000</v>
-      </c>
-      <c r="K6" s="2">
-        <v>41364</v>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="6">
+        <v>12</v>
       </c>
       <c r="M6" t="s">
         <v>526</v>
@@ -2715,10 +2736,13 @@
         <v>54</v>
       </c>
       <c r="AL6" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>72</v>
       </c>
@@ -2737,11 +2761,10 @@
       <c r="H7" s="2">
         <v>41292</v>
       </c>
-      <c r="J7" s="2">
-        <v>41000</v>
-      </c>
-      <c r="K7" s="2">
-        <v>41364</v>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="6">
+        <v>12</v>
       </c>
       <c r="M7" t="s">
         <v>527</v>
@@ -2791,10 +2814,13 @@
         <v>54</v>
       </c>
       <c r="AL7" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>76</v>
       </c>
@@ -2813,11 +2839,10 @@
       <c r="H8" s="2">
         <v>41292</v>
       </c>
-      <c r="J8" s="2">
-        <v>41000</v>
-      </c>
-      <c r="K8" s="2">
-        <v>41364</v>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="6">
+        <v>12</v>
       </c>
       <c r="M8" t="s">
         <v>528</v>
@@ -2864,10 +2889,13 @@
         <v>54</v>
       </c>
       <c r="AL8" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -2886,11 +2914,10 @@
       <c r="H9" s="2">
         <v>41292</v>
       </c>
-      <c r="J9" s="2">
-        <v>41000</v>
-      </c>
-      <c r="K9" s="2">
-        <v>41364</v>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="6">
+        <v>12</v>
       </c>
       <c r="M9" t="s">
         <v>529</v>
@@ -2940,10 +2967,13 @@
         <v>54</v>
       </c>
       <c r="AL9" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -2962,11 +2992,10 @@
       <c r="H10" s="2">
         <v>41447</v>
       </c>
-      <c r="J10" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K10" s="2">
-        <v>41729</v>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="6">
+        <v>12</v>
       </c>
       <c r="M10" t="s">
         <v>530</v>
@@ -3016,10 +3045,13 @@
         <v>54</v>
       </c>
       <c r="AL10" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM10" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>88</v>
       </c>
@@ -3038,11 +3070,10 @@
       <c r="H11" s="2">
         <v>41447</v>
       </c>
-      <c r="J11" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K11" s="2">
-        <v>41729</v>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="6">
+        <v>12</v>
       </c>
       <c r="M11" t="s">
         <v>531</v>
@@ -3089,10 +3120,13 @@
         <v>54</v>
       </c>
       <c r="AL11" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>92</v>
       </c>
@@ -3111,11 +3145,10 @@
       <c r="H12" s="2">
         <v>41447</v>
       </c>
-      <c r="J12" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K12" s="2">
-        <v>41729</v>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="6">
+        <v>12</v>
       </c>
       <c r="M12" t="s">
         <v>532</v>
@@ -3162,10 +3195,13 @@
         <v>54</v>
       </c>
       <c r="AL12" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -3184,11 +3220,10 @@
       <c r="H13" s="2">
         <v>41447</v>
       </c>
-      <c r="J13" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K13" s="2">
-        <v>41729</v>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="6">
+        <v>12</v>
       </c>
       <c r="M13" t="s">
         <v>533</v>
@@ -3235,10 +3270,13 @@
         <v>54</v>
       </c>
       <c r="AL13" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>100</v>
       </c>
@@ -3257,11 +3295,10 @@
       <c r="H14" s="2">
         <v>41447</v>
       </c>
-      <c r="J14" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K14" s="2">
-        <v>41729</v>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="6">
+        <v>12</v>
       </c>
       <c r="M14" t="s">
         <v>534</v>
@@ -3308,10 +3345,13 @@
         <v>54</v>
       </c>
       <c r="AL14" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>104</v>
       </c>
@@ -3330,11 +3370,10 @@
       <c r="H15" s="2">
         <v>41447</v>
       </c>
-      <c r="J15" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K15" s="2">
-        <v>41729</v>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="6">
+        <v>12</v>
       </c>
       <c r="M15" t="s">
         <v>535</v>
@@ -3384,10 +3423,13 @@
         <v>54</v>
       </c>
       <c r="AL15" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM15" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>108</v>
       </c>
@@ -3406,11 +3448,10 @@
       <c r="H16" s="2">
         <v>41447</v>
       </c>
-      <c r="J16" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K16" s="2">
-        <v>41729</v>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="6">
+        <v>12</v>
       </c>
       <c r="M16" t="s">
         <v>536</v>
@@ -3460,10 +3501,13 @@
         <v>54</v>
       </c>
       <c r="AL16" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM16" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>112</v>
       </c>
@@ -3482,11 +3526,10 @@
       <c r="H17" s="2">
         <v>41447</v>
       </c>
-      <c r="J17" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K17" s="2">
-        <v>41729</v>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="6">
+        <v>12</v>
       </c>
       <c r="M17" t="s">
         <v>537</v>
@@ -3536,10 +3579,13 @@
         <v>54</v>
       </c>
       <c r="AL17" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM17" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>117</v>
       </c>
@@ -3558,11 +3604,10 @@
       <c r="H18" s="2">
         <v>41447</v>
       </c>
-      <c r="J18" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K18" s="2">
-        <v>41729</v>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="6">
+        <v>12</v>
       </c>
       <c r="M18" t="s">
         <v>538</v>
@@ -3612,10 +3657,13 @@
         <v>54</v>
       </c>
       <c r="AL18" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM18" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>122</v>
       </c>
@@ -3634,11 +3682,10 @@
       <c r="H19" s="2">
         <v>41447</v>
       </c>
-      <c r="J19" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K19" s="2">
-        <v>41729</v>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="6">
+        <v>12</v>
       </c>
       <c r="M19" t="s">
         <v>539</v>
@@ -3688,10 +3735,13 @@
         <v>54</v>
       </c>
       <c r="AL19" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM19" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>127</v>
       </c>
@@ -3710,11 +3760,10 @@
       <c r="H20" s="2">
         <v>41447</v>
       </c>
-      <c r="J20" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K20" s="2">
-        <v>41729</v>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="6">
+        <v>12</v>
       </c>
       <c r="M20" t="s">
         <v>532</v>
@@ -3761,10 +3810,13 @@
         <v>54</v>
       </c>
       <c r="AL20" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM20" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>129</v>
       </c>
@@ -3783,11 +3835,10 @@
       <c r="H21" s="2">
         <v>41447</v>
       </c>
-      <c r="J21" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K21" s="2">
-        <v>41729</v>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="6">
+        <v>12</v>
       </c>
       <c r="M21" t="s">
         <v>540</v>
@@ -3837,10 +3888,13 @@
         <v>54</v>
       </c>
       <c r="AL21" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM21" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -3859,11 +3913,10 @@
       <c r="H22" s="2">
         <v>41447</v>
       </c>
-      <c r="J22" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K22" s="2">
-        <v>41729</v>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="6">
+        <v>12</v>
       </c>
       <c r="M22" t="s">
         <v>541</v>
@@ -3910,10 +3963,13 @@
         <v>54</v>
       </c>
       <c r="AL22" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM22" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>138</v>
       </c>
@@ -3932,11 +3988,10 @@
       <c r="H23" s="2">
         <v>41447</v>
       </c>
-      <c r="J23" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K23" s="2">
-        <v>41729</v>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="6">
+        <v>12</v>
       </c>
       <c r="M23" t="s">
         <v>542</v>
@@ -3983,10 +4038,13 @@
         <v>54</v>
       </c>
       <c r="AL23" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM23" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>142</v>
       </c>
@@ -4005,11 +4063,10 @@
       <c r="H24" s="2">
         <v>41447</v>
       </c>
-      <c r="J24" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K24" s="2">
-        <v>41729</v>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="6">
+        <v>12</v>
       </c>
       <c r="M24" t="s">
         <v>543</v>
@@ -4059,10 +4116,13 @@
         <v>54</v>
       </c>
       <c r="AL24" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM24" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>146</v>
       </c>
@@ -4081,11 +4141,10 @@
       <c r="H25" s="2">
         <v>41447</v>
       </c>
-      <c r="J25" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K25" s="2">
-        <v>41729</v>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="6">
+        <v>12</v>
       </c>
       <c r="M25" t="s">
         <v>544</v>
@@ -4132,10 +4191,13 @@
         <v>54</v>
       </c>
       <c r="AL25" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM25" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>150</v>
       </c>
@@ -4154,11 +4216,10 @@
       <c r="H26" s="2">
         <v>41447</v>
       </c>
-      <c r="J26" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K26" s="2">
-        <v>41729</v>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="6">
+        <v>12</v>
       </c>
       <c r="M26" t="s">
         <v>545</v>
@@ -4211,10 +4272,13 @@
         <v>54</v>
       </c>
       <c r="AL26" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM26" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>156</v>
       </c>
@@ -4233,11 +4297,10 @@
       <c r="H27" s="2">
         <v>41447</v>
       </c>
-      <c r="J27" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K27" s="2">
-        <v>41729</v>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="6">
+        <v>12</v>
       </c>
       <c r="M27" t="s">
         <v>546</v>
@@ -4284,10 +4347,13 @@
         <v>54</v>
       </c>
       <c r="AL27" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM27" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>160</v>
       </c>
@@ -4306,11 +4372,10 @@
       <c r="H28" s="2">
         <v>41447</v>
       </c>
-      <c r="J28" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K28" s="2">
-        <v>41729</v>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="6">
+        <v>12</v>
       </c>
       <c r="M28" t="s">
         <v>547</v>
@@ -4357,10 +4422,13 @@
         <v>54</v>
       </c>
       <c r="AL28" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM28" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>164</v>
       </c>
@@ -4379,11 +4447,10 @@
       <c r="H29" s="2">
         <v>41454</v>
       </c>
-      <c r="J29" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K29" s="2">
-        <v>41729</v>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="6">
+        <v>12</v>
       </c>
       <c r="M29" t="s">
         <v>548</v>
@@ -4430,10 +4497,13 @@
         <v>54</v>
       </c>
       <c r="AL29" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM29" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="30" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>168</v>
       </c>
@@ -4452,11 +4522,10 @@
       <c r="H30" s="2">
         <v>41454</v>
       </c>
-      <c r="J30" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K30" s="2">
-        <v>41729</v>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="6">
+        <v>12</v>
       </c>
       <c r="M30" t="s">
         <v>549</v>
@@ -4503,10 +4572,13 @@
         <v>54</v>
       </c>
       <c r="AL30" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM30" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="31" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>172</v>
       </c>
@@ -4525,11 +4597,10 @@
       <c r="H31" s="2">
         <v>41454</v>
       </c>
-      <c r="J31" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K31" s="2">
-        <v>41729</v>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="6">
+        <v>12</v>
       </c>
       <c r="M31" t="s">
         <v>550</v>
@@ -4579,10 +4650,13 @@
         <v>54</v>
       </c>
       <c r="AL31" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM31" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="32" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>177</v>
       </c>
@@ -4601,11 +4675,10 @@
       <c r="H32" s="2">
         <v>41454</v>
       </c>
-      <c r="J32" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K32" s="2">
-        <v>41729</v>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="6">
+        <v>12</v>
       </c>
       <c r="M32" t="s">
         <v>551</v>
@@ -4652,10 +4725,13 @@
         <v>54</v>
       </c>
       <c r="AL32" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM32" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="33" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>181</v>
       </c>
@@ -4674,11 +4750,10 @@
       <c r="H33" s="2">
         <v>41454</v>
       </c>
-      <c r="J33" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K33" s="2">
-        <v>41729</v>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="6">
+        <v>12</v>
       </c>
       <c r="M33" t="s">
         <v>552</v>
@@ -4725,10 +4800,13 @@
         <v>54</v>
       </c>
       <c r="AL33" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM33" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="34" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>185</v>
       </c>
@@ -4747,11 +4825,10 @@
       <c r="H34" s="2">
         <v>41454</v>
       </c>
-      <c r="J34" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K34" s="2">
-        <v>41729</v>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="6">
+        <v>12</v>
       </c>
       <c r="M34" t="s">
         <v>553</v>
@@ -4801,10 +4878,13 @@
         <v>54</v>
       </c>
       <c r="AL34" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM34" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="35" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>190</v>
       </c>
@@ -4823,11 +4903,10 @@
       <c r="H35" s="2">
         <v>41454</v>
       </c>
-      <c r="J35" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K35" s="2">
-        <v>41729</v>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="6">
+        <v>12</v>
       </c>
       <c r="M35" t="s">
         <v>554</v>
@@ -4874,10 +4953,13 @@
         <v>54</v>
       </c>
       <c r="AL35" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM35" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="36" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>194</v>
       </c>
@@ -4896,11 +4978,10 @@
       <c r="H36" s="2">
         <v>41454</v>
       </c>
-      <c r="J36" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K36" s="2">
-        <v>41729</v>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="6">
+        <v>12</v>
       </c>
       <c r="M36" t="s">
         <v>555</v>
@@ -4947,10 +5028,13 @@
         <v>54</v>
       </c>
       <c r="AL36" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM36" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="37" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>198</v>
       </c>
@@ -4969,11 +5053,10 @@
       <c r="H37" s="2">
         <v>41454</v>
       </c>
-      <c r="J37" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K37" s="2">
-        <v>41729</v>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="6">
+        <v>12</v>
       </c>
       <c r="M37" t="s">
         <v>536</v>
@@ -5023,10 +5106,13 @@
         <v>54</v>
       </c>
       <c r="AL37" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM37" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="38" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>200</v>
       </c>
@@ -5045,11 +5131,10 @@
       <c r="H38" s="2">
         <v>41454</v>
       </c>
-      <c r="J38" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K38" s="2">
-        <v>41729</v>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="6">
+        <v>12</v>
       </c>
       <c r="M38" t="s">
         <v>556</v>
@@ -5096,10 +5181,13 @@
         <v>54</v>
       </c>
       <c r="AL38" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM38" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="39" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>204</v>
       </c>
@@ -5118,11 +5206,10 @@
       <c r="H39" s="2">
         <v>41454</v>
       </c>
-      <c r="J39" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K39" s="2">
-        <v>41729</v>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="6">
+        <v>12</v>
       </c>
       <c r="M39" t="s">
         <v>557</v>
@@ -5169,10 +5256,13 @@
         <v>54</v>
       </c>
       <c r="AL39" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM39" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="40" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>208</v>
       </c>
@@ -5191,11 +5281,10 @@
       <c r="H40" s="2">
         <v>41454</v>
       </c>
-      <c r="J40" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K40" s="2">
-        <v>41729</v>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="6">
+        <v>12</v>
       </c>
       <c r="M40" t="s">
         <v>558</v>
@@ -5245,10 +5334,13 @@
         <v>54</v>
       </c>
       <c r="AL40" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM40" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="41" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>213</v>
       </c>
@@ -5267,11 +5359,10 @@
       <c r="H41" s="2">
         <v>41454</v>
       </c>
-      <c r="J41" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K41" s="2">
-        <v>41729</v>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="6">
+        <v>12</v>
       </c>
       <c r="M41" t="s">
         <v>559</v>
@@ -5318,10 +5409,13 @@
         <v>54</v>
       </c>
       <c r="AL41" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM41" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="42" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>217</v>
       </c>
@@ -5340,11 +5434,10 @@
       <c r="H42" s="2">
         <v>41454</v>
       </c>
-      <c r="J42" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K42" s="2">
-        <v>41729</v>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="6">
+        <v>12</v>
       </c>
       <c r="M42" t="s">
         <v>560</v>
@@ -5391,10 +5484,13 @@
         <v>54</v>
       </c>
       <c r="AL42" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM42" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="43" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>221</v>
       </c>
@@ -5413,11 +5509,10 @@
       <c r="H43" s="2">
         <v>41454</v>
       </c>
-      <c r="J43" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K43" s="2">
-        <v>41729</v>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="6">
+        <v>12</v>
       </c>
       <c r="M43" t="s">
         <v>561</v>
@@ -5464,10 +5559,13 @@
         <v>54</v>
       </c>
       <c r="AL43" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM43" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="44" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>225</v>
       </c>
@@ -5486,11 +5584,10 @@
       <c r="H44" s="2">
         <v>41454</v>
       </c>
-      <c r="J44" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K44" s="2">
-        <v>41729</v>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="6">
+        <v>12</v>
       </c>
       <c r="M44" t="s">
         <v>562</v>
@@ -5537,10 +5634,13 @@
         <v>54</v>
       </c>
       <c r="AL44" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM44" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="45" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>229</v>
       </c>
@@ -5559,11 +5659,10 @@
       <c r="H45" s="2">
         <v>41454</v>
       </c>
-      <c r="J45" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K45" s="2">
-        <v>41729</v>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="6">
+        <v>12</v>
       </c>
       <c r="M45" t="s">
         <v>563</v>
@@ -5610,10 +5709,13 @@
         <v>54</v>
       </c>
       <c r="AL45" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM45" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="46" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>233</v>
       </c>
@@ -5632,11 +5734,10 @@
       <c r="H46" s="2">
         <v>41454</v>
       </c>
-      <c r="J46" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K46" s="2">
-        <v>41729</v>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="6">
+        <v>12</v>
       </c>
       <c r="M46" t="s">
         <v>564</v>
@@ -5683,10 +5784,13 @@
         <v>54</v>
       </c>
       <c r="AL46" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM46" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="47" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>237</v>
       </c>
@@ -5705,11 +5809,10 @@
       <c r="H47" s="2">
         <v>41454</v>
       </c>
-      <c r="J47" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K47" s="2">
-        <v>41729</v>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="6">
+        <v>12</v>
       </c>
       <c r="M47" t="s">
         <v>565</v>
@@ -5762,10 +5865,13 @@
         <v>54</v>
       </c>
       <c r="AL47" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM47" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="48" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>242</v>
       </c>
@@ -5784,11 +5890,10 @@
       <c r="H48" s="2">
         <v>41454</v>
       </c>
-      <c r="J48" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K48" s="2">
-        <v>41729</v>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="6">
+        <v>12</v>
       </c>
       <c r="M48" t="s">
         <v>565</v>
@@ -5841,10 +5946,13 @@
         <v>54</v>
       </c>
       <c r="AL48" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM48" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="49" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>245</v>
       </c>
@@ -5863,11 +5971,10 @@
       <c r="H49" s="2">
         <v>41454</v>
       </c>
-      <c r="J49" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K49" s="2">
-        <v>41729</v>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="6">
+        <v>12</v>
       </c>
       <c r="M49" t="s">
         <v>566</v>
@@ -5914,10 +6021,13 @@
         <v>54</v>
       </c>
       <c r="AL49" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM49" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="50" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>249</v>
       </c>
@@ -5936,11 +6046,10 @@
       <c r="H50" s="2">
         <v>41454</v>
       </c>
-      <c r="J50" s="2">
-        <v>41365</v>
-      </c>
-      <c r="K50" s="2">
-        <v>41729</v>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="6">
+        <v>12</v>
       </c>
       <c r="M50" t="s">
         <v>567</v>
@@ -5987,10 +6096,13 @@
         <v>54</v>
       </c>
       <c r="AL50" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM50" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="51" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>253</v>
       </c>
@@ -6009,11 +6121,10 @@
       <c r="H51" s="2">
         <v>41825</v>
       </c>
-      <c r="J51" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K51" s="2">
-        <v>42094</v>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="6">
+        <v>12</v>
       </c>
       <c r="M51" t="s">
         <v>568</v>
@@ -6060,10 +6171,13 @@
         <v>54</v>
       </c>
       <c r="AL51" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="52" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM51" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="52" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>257</v>
       </c>
@@ -6082,11 +6196,10 @@
       <c r="H52" s="2">
         <v>41825</v>
       </c>
-      <c r="J52" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K52" s="2">
-        <v>42094</v>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="6">
+        <v>12</v>
       </c>
       <c r="M52" t="s">
         <v>569</v>
@@ -6139,10 +6252,13 @@
         <v>54</v>
       </c>
       <c r="AL52" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="53" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM52" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="53" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>263</v>
       </c>
@@ -6161,11 +6277,10 @@
       <c r="H53" s="2">
         <v>41825</v>
       </c>
-      <c r="J53" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K53" s="2">
-        <v>42094</v>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="6">
+        <v>12</v>
       </c>
       <c r="M53" t="s">
         <v>570</v>
@@ -6212,10 +6327,13 @@
         <v>54</v>
       </c>
       <c r="AL53" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="54" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM53" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="54" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>267</v>
       </c>
@@ -6234,11 +6352,10 @@
       <c r="H54" s="2">
         <v>41825</v>
       </c>
-      <c r="J54" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K54" s="2">
-        <v>42094</v>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="6">
+        <v>12</v>
       </c>
       <c r="M54" t="s">
         <v>571</v>
@@ -6285,10 +6402,13 @@
         <v>54</v>
       </c>
       <c r="AL54" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="55" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM54" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="55" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>271</v>
       </c>
@@ -6307,11 +6427,10 @@
       <c r="H55" s="2">
         <v>41825</v>
       </c>
-      <c r="J55" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K55" s="2">
-        <v>42094</v>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="6">
+        <v>12</v>
       </c>
       <c r="M55" t="s">
         <v>550</v>
@@ -6361,10 +6480,13 @@
         <v>54</v>
       </c>
       <c r="AL55" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="56" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM55" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="56" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>273</v>
       </c>
@@ -6383,11 +6505,10 @@
       <c r="H56" s="2">
         <v>41825</v>
       </c>
-      <c r="J56" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K56" s="2">
-        <v>42094</v>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="6">
+        <v>12</v>
       </c>
       <c r="M56" t="s">
         <v>572</v>
@@ -6437,10 +6558,13 @@
         <v>54</v>
       </c>
       <c r="AL56" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="57" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM56" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="57" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>278</v>
       </c>
@@ -6459,11 +6583,10 @@
       <c r="H57" s="2">
         <v>41825</v>
       </c>
-      <c r="J57" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K57" s="2">
-        <v>42094</v>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="6">
+        <v>12</v>
       </c>
       <c r="M57" t="s">
         <v>573</v>
@@ -6510,10 +6633,13 @@
         <v>54</v>
       </c>
       <c r="AL57" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="58" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM57" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="58" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>282</v>
       </c>
@@ -6532,11 +6658,10 @@
       <c r="H58" s="2">
         <v>41825</v>
       </c>
-      <c r="J58" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K58" s="2">
-        <v>42094</v>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+      <c r="L58" s="6">
+        <v>12</v>
       </c>
       <c r="M58" t="s">
         <v>574</v>
@@ -6583,10 +6708,13 @@
         <v>54</v>
       </c>
       <c r="AL58" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="59" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM58" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="59" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>286</v>
       </c>
@@ -6605,11 +6733,10 @@
       <c r="H59" s="2">
         <v>41832</v>
       </c>
-      <c r="J59" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K59" s="2">
-        <v>42094</v>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+      <c r="L59" s="6">
+        <v>12</v>
       </c>
       <c r="M59" t="s">
         <v>575</v>
@@ -6656,10 +6783,13 @@
         <v>54</v>
       </c>
       <c r="AL59" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="60" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM59" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="60" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>290</v>
       </c>
@@ -6678,11 +6808,10 @@
       <c r="H60" s="2">
         <v>41832</v>
       </c>
-      <c r="J60" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K60" s="2">
-        <v>42094</v>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+      <c r="L60" s="6">
+        <v>12</v>
       </c>
       <c r="M60" t="s">
         <v>560</v>
@@ -6729,10 +6858,13 @@
         <v>54</v>
       </c>
       <c r="AL60" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="61" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM60" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="61" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>292</v>
       </c>
@@ -6751,11 +6883,10 @@
       <c r="H61" s="2">
         <v>41832</v>
       </c>
-      <c r="J61" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K61" s="2">
-        <v>42094</v>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="6">
+        <v>12</v>
       </c>
       <c r="M61" t="s">
         <v>576</v>
@@ -6805,10 +6936,13 @@
         <v>54</v>
       </c>
       <c r="AL61" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="62" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM61" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="62" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>296</v>
       </c>
@@ -6827,11 +6961,10 @@
       <c r="H62" s="2">
         <v>41832</v>
       </c>
-      <c r="J62" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K62" s="2">
-        <v>42094</v>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="6">
+        <v>12</v>
       </c>
       <c r="M62" t="s">
         <v>577</v>
@@ -6878,10 +7011,13 @@
         <v>54</v>
       </c>
       <c r="AL62" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="63" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM62" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="63" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>300</v>
       </c>
@@ -6900,11 +7036,10 @@
       <c r="H63" s="2">
         <v>41832</v>
       </c>
-      <c r="J63" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K63" s="2">
-        <v>42094</v>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="6">
+        <v>12</v>
       </c>
       <c r="M63" t="s">
         <v>578</v>
@@ -6957,10 +7092,13 @@
         <v>54</v>
       </c>
       <c r="AL63" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="64" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM63" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="64" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>306</v>
       </c>
@@ -6979,11 +7117,10 @@
       <c r="H64" s="2">
         <v>41832</v>
       </c>
-      <c r="J64" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K64" s="2">
-        <v>42094</v>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="6">
+        <v>12</v>
       </c>
       <c r="M64" t="s">
         <v>579</v>
@@ -7030,10 +7167,13 @@
         <v>54</v>
       </c>
       <c r="AL64" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="65" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM64" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="65" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>310</v>
       </c>
@@ -7052,11 +7192,10 @@
       <c r="H65" s="2">
         <v>41832</v>
       </c>
-      <c r="J65" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K65" s="2">
-        <v>42094</v>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="6">
+        <v>12</v>
       </c>
       <c r="M65" t="s">
         <v>550</v>
@@ -7106,10 +7245,13 @@
         <v>54</v>
       </c>
       <c r="AL65" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="66" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM65" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="66" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>312</v>
       </c>
@@ -7128,11 +7270,10 @@
       <c r="H66" s="2">
         <v>41832</v>
       </c>
-      <c r="J66" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K66" s="2">
-        <v>42094</v>
+      <c r="J66" s="2"/>
+      <c r="K66" s="2"/>
+      <c r="L66" s="6">
+        <v>12</v>
       </c>
       <c r="M66" t="s">
         <v>580</v>
@@ -7179,10 +7320,13 @@
         <v>54</v>
       </c>
       <c r="AL66" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="67" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM66" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="67" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>316</v>
       </c>
@@ -7201,11 +7345,10 @@
       <c r="H67" s="2">
         <v>41832</v>
       </c>
-      <c r="J67" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K67" s="2">
-        <v>42094</v>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2"/>
+      <c r="L67" s="6">
+        <v>12</v>
       </c>
       <c r="M67" t="s">
         <v>581</v>
@@ -7252,10 +7395,13 @@
         <v>54</v>
       </c>
       <c r="AL67" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="68" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM67" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="68" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>320</v>
       </c>
@@ -7274,11 +7420,10 @@
       <c r="H68" s="2">
         <v>41832</v>
       </c>
-      <c r="J68" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K68" s="2">
-        <v>42094</v>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="6">
+        <v>12</v>
       </c>
       <c r="M68" t="s">
         <v>536</v>
@@ -7328,10 +7473,13 @@
         <v>54</v>
       </c>
       <c r="AL68" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="69" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM68" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="69" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>322</v>
       </c>
@@ -7350,11 +7498,10 @@
       <c r="H69" s="2">
         <v>41839</v>
       </c>
-      <c r="J69" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K69" s="2">
-        <v>42094</v>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="6">
+        <v>12</v>
       </c>
       <c r="M69" t="s">
         <v>525</v>
@@ -7407,10 +7554,13 @@
         <v>54</v>
       </c>
       <c r="AL69" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="70" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM69" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="70" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>324</v>
       </c>
@@ -7429,11 +7579,10 @@
       <c r="H70" s="2">
         <v>41839</v>
       </c>
-      <c r="J70" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K70" s="2">
-        <v>42094</v>
+      <c r="J70" s="2"/>
+      <c r="K70" s="2"/>
+      <c r="L70" s="6">
+        <v>12</v>
       </c>
       <c r="M70" t="s">
         <v>575</v>
@@ -7480,10 +7629,13 @@
         <v>54</v>
       </c>
       <c r="AL70" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="71" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM70" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="71" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>326</v>
       </c>
@@ -7502,11 +7654,10 @@
       <c r="H71" s="2">
         <v>41839</v>
       </c>
-      <c r="J71" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K71" s="2">
-        <v>42094</v>
+      <c r="J71" s="2"/>
+      <c r="K71" s="2"/>
+      <c r="L71" s="6">
+        <v>12</v>
       </c>
       <c r="M71" t="s">
         <v>529</v>
@@ -7556,10 +7707,13 @@
         <v>54</v>
       </c>
       <c r="AL71" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="72" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM71" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="72" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>328</v>
       </c>
@@ -7578,11 +7732,10 @@
       <c r="H72" s="2">
         <v>41839</v>
       </c>
-      <c r="J72" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K72" s="2">
-        <v>42094</v>
+      <c r="J72" s="2"/>
+      <c r="K72" s="2"/>
+      <c r="L72" s="6">
+        <v>12</v>
       </c>
       <c r="M72" t="s">
         <v>582</v>
@@ -7629,10 +7782,13 @@
         <v>54</v>
       </c>
       <c r="AL72" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="73" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM72" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="73" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>332</v>
       </c>
@@ -7651,11 +7807,10 @@
       <c r="H73" s="2">
         <v>41839</v>
       </c>
-      <c r="J73" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K73" s="2">
-        <v>42094</v>
+      <c r="J73" s="2"/>
+      <c r="K73" s="2"/>
+      <c r="L73" s="6">
+        <v>12</v>
       </c>
       <c r="M73" t="s">
         <v>583</v>
@@ -7705,10 +7860,13 @@
         <v>54</v>
       </c>
       <c r="AL73" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="74" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM73" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="74" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>337</v>
       </c>
@@ -7727,11 +7885,10 @@
       <c r="H74" s="2">
         <v>41839</v>
       </c>
-      <c r="J74" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K74" s="2">
-        <v>42094</v>
+      <c r="J74" s="2"/>
+      <c r="K74" s="2"/>
+      <c r="L74" s="6">
+        <v>12</v>
       </c>
       <c r="M74" t="s">
         <v>584</v>
@@ -7778,10 +7935,13 @@
         <v>54</v>
       </c>
       <c r="AL74" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="75" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM74" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="75" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>341</v>
       </c>
@@ -7800,11 +7960,10 @@
       <c r="H75" s="2">
         <v>41839</v>
       </c>
-      <c r="J75" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K75" s="2">
-        <v>42094</v>
+      <c r="J75" s="2"/>
+      <c r="K75" s="2"/>
+      <c r="L75" s="6">
+        <v>12</v>
       </c>
       <c r="M75" t="s">
         <v>530</v>
@@ -7854,10 +8013,13 @@
         <v>54</v>
       </c>
       <c r="AL75" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="76" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM75" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="76" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>343</v>
       </c>
@@ -7876,11 +8038,10 @@
       <c r="H76" s="2">
         <v>41839</v>
       </c>
-      <c r="J76" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K76" s="2">
-        <v>42094</v>
+      <c r="J76" s="2"/>
+      <c r="K76" s="2"/>
+      <c r="L76" s="6">
+        <v>12</v>
       </c>
       <c r="M76" t="s">
         <v>585</v>
@@ -7927,10 +8088,13 @@
         <v>54</v>
       </c>
       <c r="AL76" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="77" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM76" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="77" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>347</v>
       </c>
@@ -7949,11 +8113,10 @@
       <c r="H77" s="2">
         <v>41888</v>
       </c>
-      <c r="J77" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K77" s="2">
-        <v>42094</v>
+      <c r="J77" s="2"/>
+      <c r="K77" s="2"/>
+      <c r="L77" s="6">
+        <v>12</v>
       </c>
       <c r="M77" t="s">
         <v>568</v>
@@ -8000,10 +8163,13 @@
         <v>54</v>
       </c>
       <c r="AL77" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="78" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM77" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="78" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>349</v>
       </c>
@@ -8022,11 +8188,10 @@
       <c r="H78" s="2">
         <v>41888</v>
       </c>
-      <c r="J78" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K78" s="2">
-        <v>42094</v>
+      <c r="J78" s="2"/>
+      <c r="K78" s="2"/>
+      <c r="L78" s="6">
+        <v>12</v>
       </c>
       <c r="M78" t="s">
         <v>586</v>
@@ -8073,10 +8238,13 @@
         <v>54</v>
       </c>
       <c r="AL78" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="79" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM78" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="79" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>353</v>
       </c>
@@ -8095,11 +8263,10 @@
       <c r="H79" s="2">
         <v>41888</v>
       </c>
-      <c r="J79" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K79" s="2">
-        <v>42094</v>
+      <c r="J79" s="2"/>
+      <c r="K79" s="2"/>
+      <c r="L79" s="6">
+        <v>12</v>
       </c>
       <c r="M79" t="s">
         <v>587</v>
@@ -8146,10 +8313,13 @@
         <v>54</v>
       </c>
       <c r="AL79" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="80" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM79" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="80" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>357</v>
       </c>
@@ -8168,11 +8338,10 @@
       <c r="H80" s="2">
         <v>41888</v>
       </c>
-      <c r="J80" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K80" s="2">
-        <v>42094</v>
+      <c r="J80" s="2"/>
+      <c r="K80" s="2"/>
+      <c r="L80" s="6">
+        <v>12</v>
       </c>
       <c r="M80" t="s">
         <v>588</v>
@@ -8225,10 +8394,13 @@
         <v>54</v>
       </c>
       <c r="AL80" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="81" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM80" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="81" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>363</v>
       </c>
@@ -8247,11 +8419,10 @@
       <c r="H81" s="2">
         <v>41888</v>
       </c>
-      <c r="J81" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K81" s="2">
-        <v>42094</v>
+      <c r="J81" s="2"/>
+      <c r="K81" s="2"/>
+      <c r="L81" s="6">
+        <v>12</v>
       </c>
       <c r="M81" t="s">
         <v>589</v>
@@ -8304,10 +8475,13 @@
         <v>54</v>
       </c>
       <c r="AL81" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="82" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM81" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="82" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>369</v>
       </c>
@@ -8326,11 +8500,10 @@
       <c r="H82" s="2">
         <v>41888</v>
       </c>
-      <c r="J82" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K82" s="2">
-        <v>42094</v>
+      <c r="J82" s="2"/>
+      <c r="K82" s="2"/>
+      <c r="L82" s="6">
+        <v>12</v>
       </c>
       <c r="M82" t="s">
         <v>532</v>
@@ -8377,10 +8550,13 @@
         <v>54</v>
       </c>
       <c r="AL82" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="83" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM82" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="83" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>371</v>
       </c>
@@ -8399,11 +8575,10 @@
       <c r="H83" s="2">
         <v>41888</v>
       </c>
-      <c r="J83" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K83" s="2">
-        <v>42094</v>
+      <c r="J83" s="2"/>
+      <c r="K83" s="2"/>
+      <c r="L83" s="6">
+        <v>12</v>
       </c>
       <c r="M83" t="s">
         <v>590</v>
@@ -8450,10 +8625,13 @@
         <v>54</v>
       </c>
       <c r="AL83" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="84" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM83" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="84" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>375</v>
       </c>
@@ -8472,11 +8650,10 @@
       <c r="H84" s="2">
         <v>41888</v>
       </c>
-      <c r="J84" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K84" s="2">
-        <v>42094</v>
+      <c r="J84" s="2"/>
+      <c r="K84" s="2"/>
+      <c r="L84" s="6">
+        <v>12</v>
       </c>
       <c r="M84" t="s">
         <v>591</v>
@@ -8523,10 +8700,13 @@
         <v>54</v>
       </c>
       <c r="AL84" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="85" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM84" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="85" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>379</v>
       </c>
@@ -8545,11 +8725,10 @@
       <c r="H85" s="2">
         <v>41888</v>
       </c>
-      <c r="J85" s="2">
-        <v>41730</v>
-      </c>
-      <c r="K85" s="2">
-        <v>42094</v>
+      <c r="J85" s="2"/>
+      <c r="K85" s="2"/>
+      <c r="L85" s="6">
+        <v>12</v>
       </c>
       <c r="M85" t="s">
         <v>592</v>
@@ -8596,10 +8775,13 @@
         <v>54</v>
       </c>
       <c r="AL85" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="86" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM85" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="86" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>383</v>
       </c>
@@ -8618,13 +8800,11 @@
       <c r="H86" s="3">
         <v>42896</v>
       </c>
-      <c r="J86" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K86" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L86" s="1"/>
+      <c r="J86" s="3"/>
+      <c r="K86" s="3"/>
+      <c r="L86" s="6">
+        <v>12</v>
+      </c>
       <c r="M86" t="s">
         <v>555</v>
       </c>
@@ -8670,10 +8850,13 @@
         <v>54</v>
       </c>
       <c r="AL86" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="87" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM86" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="87" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>386</v>
       </c>
@@ -8692,13 +8875,11 @@
       <c r="H87" s="3">
         <v>42896</v>
       </c>
-      <c r="J87" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K87" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L87" s="1"/>
+      <c r="J87" s="3"/>
+      <c r="K87" s="3"/>
+      <c r="L87" s="6">
+        <v>12</v>
+      </c>
       <c r="M87" t="s">
         <v>593</v>
       </c>
@@ -8744,10 +8925,13 @@
         <v>54</v>
       </c>
       <c r="AL87" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="88" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM87" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="88" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>390</v>
       </c>
@@ -8766,13 +8950,11 @@
       <c r="H88" s="3">
         <v>42896</v>
       </c>
-      <c r="J88" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K88" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L88" s="1"/>
+      <c r="J88" s="3"/>
+      <c r="K88" s="3"/>
+      <c r="L88" s="6">
+        <v>12</v>
+      </c>
       <c r="M88" t="s">
         <v>594</v>
       </c>
@@ -8818,10 +9000,13 @@
         <v>54</v>
       </c>
       <c r="AL88" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="89" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM88" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="89" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>394</v>
       </c>
@@ -8840,13 +9025,11 @@
       <c r="H89" s="3">
         <v>42896</v>
       </c>
-      <c r="J89" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K89" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L89" s="1"/>
+      <c r="J89" s="3"/>
+      <c r="K89" s="3"/>
+      <c r="L89" s="6">
+        <v>12</v>
+      </c>
       <c r="M89" t="s">
         <v>595</v>
       </c>
@@ -8892,10 +9075,13 @@
         <v>54</v>
       </c>
       <c r="AL89" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="90" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM89" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="90" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>398</v>
       </c>
@@ -8914,13 +9100,11 @@
       <c r="H90" s="3">
         <v>42896</v>
       </c>
-      <c r="J90" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K90" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L90" s="1"/>
+      <c r="J90" s="3"/>
+      <c r="K90" s="3"/>
+      <c r="L90" s="6">
+        <v>12</v>
+      </c>
       <c r="M90" t="s">
         <v>596</v>
       </c>
@@ -8966,10 +9150,13 @@
         <v>54</v>
       </c>
       <c r="AL90" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="91" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM90" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="91" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>402</v>
       </c>
@@ -8988,13 +9175,11 @@
       <c r="H91" s="3">
         <v>42896</v>
       </c>
-      <c r="J91" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K91" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L91" s="1"/>
+      <c r="J91" s="3"/>
+      <c r="K91" s="3"/>
+      <c r="L91" s="6">
+        <v>12</v>
+      </c>
       <c r="M91" t="s">
         <v>597</v>
       </c>
@@ -9043,10 +9228,13 @@
         <v>54</v>
       </c>
       <c r="AL91" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="92" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM91" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="92" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>407</v>
       </c>
@@ -9065,13 +9253,11 @@
       <c r="H92" s="3">
         <v>42903</v>
       </c>
-      <c r="J92" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K92" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L92" s="1"/>
+      <c r="J92" s="3"/>
+      <c r="K92" s="3"/>
+      <c r="L92" s="6">
+        <v>12</v>
+      </c>
       <c r="M92" t="s">
         <v>529</v>
       </c>
@@ -9120,10 +9306,13 @@
         <v>54</v>
       </c>
       <c r="AL92" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="93" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM92" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="93" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>410</v>
       </c>
@@ -9142,13 +9331,11 @@
       <c r="H93" s="3">
         <v>42903</v>
       </c>
-      <c r="J93" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K93" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L93" s="1"/>
+      <c r="J93" s="3"/>
+      <c r="K93" s="3"/>
+      <c r="L93" s="6">
+        <v>12</v>
+      </c>
       <c r="M93" t="s">
         <v>530</v>
       </c>
@@ -9197,10 +9384,13 @@
         <v>54</v>
       </c>
       <c r="AL93" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="94" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM93" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="94" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>413</v>
       </c>
@@ -9219,13 +9409,11 @@
       <c r="H94" s="3">
         <v>42903</v>
       </c>
-      <c r="J94" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K94" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L94" s="1"/>
+      <c r="J94" s="3"/>
+      <c r="K94" s="3"/>
+      <c r="L94" s="6">
+        <v>12</v>
+      </c>
       <c r="M94" t="s">
         <v>576</v>
       </c>
@@ -9274,10 +9462,13 @@
         <v>54</v>
       </c>
       <c r="AL94" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="95" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM94" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="95" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>416</v>
       </c>
@@ -9296,13 +9487,11 @@
       <c r="H95" s="3">
         <v>42903</v>
       </c>
-      <c r="J95" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K95" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L95" s="1"/>
+      <c r="J95" s="3"/>
+      <c r="K95" s="3"/>
+      <c r="L95" s="6">
+        <v>12</v>
+      </c>
       <c r="M95" t="s">
         <v>569</v>
       </c>
@@ -9354,10 +9543,13 @@
         <v>54</v>
       </c>
       <c r="AL95" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="96" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM95" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="96" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>419</v>
       </c>
@@ -9376,13 +9568,11 @@
       <c r="H96" s="3">
         <v>42903</v>
       </c>
-      <c r="J96" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K96" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L96" s="1"/>
+      <c r="J96" s="3"/>
+      <c r="K96" s="3"/>
+      <c r="L96" s="6">
+        <v>12</v>
+      </c>
       <c r="M96" t="s">
         <v>598</v>
       </c>
@@ -9431,10 +9621,13 @@
         <v>54</v>
       </c>
       <c r="AL96" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="97" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM96" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="97" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>424</v>
       </c>
@@ -9453,13 +9646,11 @@
       <c r="H97" s="3">
         <v>42903</v>
       </c>
-      <c r="J97" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K97" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L97" s="1"/>
+      <c r="J97" s="3"/>
+      <c r="K97" s="3"/>
+      <c r="L97" s="6">
+        <v>12</v>
+      </c>
       <c r="M97" t="s">
         <v>599</v>
       </c>
@@ -9511,10 +9702,13 @@
         <v>54</v>
       </c>
       <c r="AL97" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="98" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM97" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="98" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>430</v>
       </c>
@@ -9533,13 +9727,11 @@
       <c r="H98" s="3">
         <v>42903</v>
       </c>
-      <c r="J98" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K98" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L98" s="1"/>
+      <c r="J98" s="3"/>
+      <c r="K98" s="3"/>
+      <c r="L98" s="6">
+        <v>12</v>
+      </c>
       <c r="M98" t="s">
         <v>600</v>
       </c>
@@ -9585,10 +9777,13 @@
         <v>54</v>
       </c>
       <c r="AL98" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="99" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM98" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="99" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>434</v>
       </c>
@@ -9607,13 +9802,11 @@
       <c r="H99" s="3">
         <v>42903</v>
       </c>
-      <c r="J99" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K99" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L99" s="1"/>
+      <c r="J99" s="3"/>
+      <c r="K99" s="3"/>
+      <c r="L99" s="6">
+        <v>12</v>
+      </c>
       <c r="M99" t="s">
         <v>601</v>
       </c>
@@ -9662,10 +9855,13 @@
         <v>54</v>
       </c>
       <c r="AL99" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="100" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM99" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="100" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>439</v>
       </c>
@@ -9684,13 +9880,11 @@
       <c r="H100" s="3">
         <v>42903</v>
       </c>
-      <c r="J100" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K100" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L100" s="1"/>
+      <c r="J100" s="3"/>
+      <c r="K100" s="3"/>
+      <c r="L100" s="6">
+        <v>12</v>
+      </c>
       <c r="M100" t="s">
         <v>602</v>
       </c>
@@ -9739,10 +9933,13 @@
         <v>54</v>
       </c>
       <c r="AL100" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="101" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM100" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="101" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>444</v>
       </c>
@@ -9761,13 +9958,11 @@
       <c r="H101" s="3">
         <v>42903</v>
       </c>
-      <c r="J101" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K101" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L101" s="1"/>
+      <c r="J101" s="3"/>
+      <c r="K101" s="3"/>
+      <c r="L101" s="6">
+        <v>12</v>
+      </c>
       <c r="M101" t="s">
         <v>603</v>
       </c>
@@ -9819,10 +10014,13 @@
         <v>54</v>
       </c>
       <c r="AL101" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="102" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM101" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="102" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>450</v>
       </c>
@@ -9841,13 +10039,11 @@
       <c r="H102" s="3">
         <v>42904</v>
       </c>
-      <c r="J102" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K102" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L102" s="1"/>
+      <c r="J102" s="3"/>
+      <c r="K102" s="3"/>
+      <c r="L102" s="6">
+        <v>12</v>
+      </c>
       <c r="M102" t="s">
         <v>587</v>
       </c>
@@ -9893,10 +10089,13 @@
         <v>54</v>
       </c>
       <c r="AL102" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="103" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM102" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="103" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>452</v>
       </c>
@@ -9915,13 +10114,11 @@
       <c r="H103" s="3">
         <v>42904</v>
       </c>
-      <c r="J103" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K103" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L103" s="1"/>
+      <c r="J103" s="3"/>
+      <c r="K103" s="3"/>
+      <c r="L103" s="6">
+        <v>12</v>
+      </c>
       <c r="M103" t="s">
         <v>525</v>
       </c>
@@ -9973,10 +10170,13 @@
         <v>54</v>
       </c>
       <c r="AL103" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="104" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM103" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="104" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>455</v>
       </c>
@@ -9995,13 +10195,11 @@
       <c r="H104" s="3">
         <v>42904</v>
       </c>
-      <c r="J104" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K104" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L104" s="1"/>
+      <c r="J104" s="3"/>
+      <c r="K104" s="3"/>
+      <c r="L104" s="6">
+        <v>12</v>
+      </c>
       <c r="M104" t="s">
         <v>589</v>
       </c>
@@ -10053,10 +10251,13 @@
         <v>54</v>
       </c>
       <c r="AL104" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="105" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM104" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="105" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>457</v>
       </c>
@@ -10075,13 +10276,11 @@
       <c r="H105" s="3">
         <v>42904</v>
       </c>
-      <c r="J105" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K105" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L105" s="1"/>
+      <c r="J105" s="3"/>
+      <c r="K105" s="3"/>
+      <c r="L105" s="6">
+        <v>12</v>
+      </c>
       <c r="M105" t="s">
         <v>588</v>
       </c>
@@ -10133,10 +10332,13 @@
         <v>54</v>
       </c>
       <c r="AL105" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="106" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM105" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="106" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>459</v>
       </c>
@@ -10155,13 +10357,11 @@
       <c r="H106" s="3">
         <v>42904</v>
       </c>
-      <c r="J106" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K106" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L106" s="1"/>
+      <c r="J106" s="3"/>
+      <c r="K106" s="3"/>
+      <c r="L106" s="6">
+        <v>12</v>
+      </c>
       <c r="M106" t="s">
         <v>537</v>
       </c>
@@ -10210,10 +10410,13 @@
         <v>54</v>
       </c>
       <c r="AL106" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="107" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM106" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="107" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>461</v>
       </c>
@@ -10232,13 +10435,11 @@
       <c r="H107" s="3">
         <v>42904</v>
       </c>
-      <c r="J107" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K107" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L107" s="1"/>
+      <c r="J107" s="3"/>
+      <c r="K107" s="3"/>
+      <c r="L107" s="6">
+        <v>12</v>
+      </c>
       <c r="M107" t="s">
         <v>604</v>
       </c>
@@ -10284,10 +10485,13 @@
         <v>54</v>
       </c>
       <c r="AL107" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="108" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM107" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="108" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>464</v>
       </c>
@@ -10306,13 +10510,11 @@
       <c r="H108" s="3">
         <v>42904</v>
       </c>
-      <c r="J108" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K108" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L108" s="1"/>
+      <c r="J108" s="3"/>
+      <c r="K108" s="3"/>
+      <c r="L108" s="6">
+        <v>12</v>
+      </c>
       <c r="M108" t="s">
         <v>605</v>
       </c>
@@ -10358,10 +10560,13 @@
         <v>54</v>
       </c>
       <c r="AL108" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="109" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM108" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="109" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>468</v>
       </c>
@@ -10380,13 +10585,11 @@
       <c r="H109" s="3">
         <v>42904</v>
       </c>
-      <c r="J109" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K109" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L109" s="1"/>
+      <c r="J109" s="3"/>
+      <c r="K109" s="3"/>
+      <c r="L109" s="6">
+        <v>12</v>
+      </c>
       <c r="M109" t="s">
         <v>606</v>
       </c>
@@ -10432,10 +10635,13 @@
         <v>54</v>
       </c>
       <c r="AL109" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="110" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM109" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="110" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>472</v>
       </c>
@@ -10454,13 +10660,11 @@
       <c r="H110" s="3">
         <v>42904</v>
       </c>
-      <c r="J110" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K110" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L110" s="1"/>
+      <c r="J110" s="3"/>
+      <c r="K110" s="3"/>
+      <c r="L110" s="6">
+        <v>12</v>
+      </c>
       <c r="M110" t="s">
         <v>607</v>
       </c>
@@ -10506,10 +10710,13 @@
         <v>54</v>
       </c>
       <c r="AL110" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="111" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM110" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="111" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>476</v>
       </c>
@@ -10528,13 +10735,11 @@
       <c r="H111" s="3">
         <v>42904</v>
       </c>
-      <c r="J111" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K111" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L111" s="1"/>
+      <c r="J111" s="3"/>
+      <c r="K111" s="3"/>
+      <c r="L111" s="6">
+        <v>12</v>
+      </c>
       <c r="M111" t="s">
         <v>608</v>
       </c>
@@ -10580,10 +10785,13 @@
         <v>54</v>
       </c>
       <c r="AL111" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="112" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM111" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="112" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>480</v>
       </c>
@@ -10602,13 +10810,11 @@
       <c r="H112" s="3">
         <v>42904</v>
       </c>
-      <c r="J112" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K112" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L112" s="1"/>
+      <c r="J112" s="3"/>
+      <c r="K112" s="3"/>
+      <c r="L112" s="6">
+        <v>12</v>
+      </c>
       <c r="M112" t="s">
         <v>609</v>
       </c>
@@ -10657,10 +10863,13 @@
         <v>54</v>
       </c>
       <c r="AL112" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="113" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM112" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="113" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>485</v>
       </c>
@@ -10679,13 +10888,11 @@
       <c r="H113" s="3">
         <v>42910</v>
       </c>
-      <c r="J113" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K113" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L113" s="1"/>
+      <c r="J113" s="3"/>
+      <c r="K113" s="3"/>
+      <c r="L113" s="6">
+        <v>12</v>
+      </c>
       <c r="M113" t="s">
         <v>567</v>
       </c>
@@ -10731,10 +10938,13 @@
         <v>54</v>
       </c>
       <c r="AL113" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="114" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM113" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="114" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>487</v>
       </c>
@@ -10753,13 +10963,11 @@
       <c r="H114" s="3">
         <v>42910</v>
       </c>
-      <c r="J114" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K114" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L114" s="1"/>
+      <c r="J114" s="3"/>
+      <c r="K114" s="3"/>
+      <c r="L114" s="6">
+        <v>12</v>
+      </c>
       <c r="M114" t="s">
         <v>565</v>
       </c>
@@ -10811,10 +11019,13 @@
         <v>54</v>
       </c>
       <c r="AL114" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="115" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM114" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="115" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>491</v>
       </c>
@@ -10833,13 +11044,11 @@
       <c r="H115" s="3">
         <v>42910</v>
       </c>
-      <c r="J115" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K115" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L115" s="1"/>
+      <c r="J115" s="3"/>
+      <c r="K115" s="3"/>
+      <c r="L115" s="6">
+        <v>12</v>
+      </c>
       <c r="M115" t="s">
         <v>576</v>
       </c>
@@ -10888,10 +11097,13 @@
         <v>54</v>
       </c>
       <c r="AL115" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="116" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM115" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="116" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>493</v>
       </c>
@@ -10910,13 +11122,11 @@
       <c r="H116" s="3">
         <v>42910</v>
       </c>
-      <c r="J116" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K116" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L116" s="1"/>
+      <c r="J116" s="3"/>
+      <c r="K116" s="3"/>
+      <c r="L116" s="6">
+        <v>12</v>
+      </c>
       <c r="M116" t="s">
         <v>569</v>
       </c>
@@ -10968,10 +11178,13 @@
         <v>54</v>
       </c>
       <c r="AL116" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="117" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM116" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="117" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>495</v>
       </c>
@@ -10990,13 +11203,11 @@
       <c r="H117" s="3">
         <v>42910</v>
       </c>
-      <c r="J117" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K117" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L117" s="1"/>
+      <c r="J117" s="3"/>
+      <c r="K117" s="3"/>
+      <c r="L117" s="6">
+        <v>12</v>
+      </c>
       <c r="M117" t="s">
         <v>589</v>
       </c>
@@ -11048,10 +11259,13 @@
         <v>54</v>
       </c>
       <c r="AL117" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="118" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM117" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="118" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>497</v>
       </c>
@@ -11070,13 +11284,11 @@
       <c r="H118" s="3">
         <v>42910</v>
       </c>
-      <c r="J118" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K118" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L118" s="1"/>
+      <c r="J118" s="3"/>
+      <c r="K118" s="3"/>
+      <c r="L118" s="6">
+        <v>12</v>
+      </c>
       <c r="M118" t="s">
         <v>610</v>
       </c>
@@ -11122,10 +11334,13 @@
         <v>54</v>
       </c>
       <c r="AL118" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="119" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM118" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="119" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>501</v>
       </c>
@@ -11144,13 +11359,11 @@
       <c r="H119" s="3">
         <v>42910</v>
       </c>
-      <c r="J119" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K119" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L119" s="1"/>
+      <c r="J119" s="3"/>
+      <c r="K119" s="3"/>
+      <c r="L119" s="6">
+        <v>12</v>
+      </c>
       <c r="M119" t="s">
         <v>611</v>
       </c>
@@ -11196,10 +11409,13 @@
         <v>54</v>
       </c>
       <c r="AL119" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="120" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM119" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="120" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>505</v>
       </c>
@@ -11218,13 +11434,11 @@
       <c r="H120" s="3">
         <v>42910</v>
       </c>
-      <c r="J120" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K120" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L120" s="1"/>
+      <c r="J120" s="3"/>
+      <c r="K120" s="3"/>
+      <c r="L120" s="6">
+        <v>12</v>
+      </c>
       <c r="M120" t="s">
         <v>612</v>
       </c>
@@ -11270,10 +11484,13 @@
         <v>54</v>
       </c>
       <c r="AL120" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="121" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM120" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="121" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>509</v>
       </c>
@@ -11292,13 +11509,11 @@
       <c r="H121" s="3">
         <v>42910</v>
       </c>
-      <c r="J121" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K121" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L121" s="1"/>
+      <c r="J121" s="3"/>
+      <c r="K121" s="3"/>
+      <c r="L121" s="6">
+        <v>12</v>
+      </c>
       <c r="M121" t="s">
         <v>613</v>
       </c>
@@ -11347,10 +11562,13 @@
         <v>54</v>
       </c>
       <c r="AL121" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="122" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM121" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="122" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>514</v>
       </c>
@@ -11369,13 +11587,11 @@
       <c r="H122" s="3">
         <v>42910</v>
       </c>
-      <c r="J122" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K122" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L122" s="1"/>
+      <c r="J122" s="3"/>
+      <c r="K122" s="3"/>
+      <c r="L122" s="6">
+        <v>12</v>
+      </c>
       <c r="M122" t="s">
         <v>614</v>
       </c>
@@ -11421,10 +11637,13 @@
         <v>54</v>
       </c>
       <c r="AL122" s="3">
-        <v>43067</v>
-      </c>
-    </row>
-    <row r="123" spans="1:38" x14ac:dyDescent="0.25">
+        <v>44146</v>
+      </c>
+      <c r="AM122" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="123" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>518</v>
       </c>
@@ -11443,13 +11662,11 @@
       <c r="H123" s="3">
         <v>42910</v>
       </c>
-      <c r="J123" s="3">
-        <v>42826</v>
-      </c>
-      <c r="K123" s="3">
-        <v>43190</v>
-      </c>
-      <c r="L123" s="1"/>
+      <c r="J123" s="3"/>
+      <c r="K123" s="3"/>
+      <c r="L123" s="6">
+        <v>12</v>
+      </c>
       <c r="M123" t="s">
         <v>615</v>
       </c>
@@ -11495,11 +11712,116 @@
         <v>54</v>
       </c>
       <c r="AL123" s="3">
-        <v>43067</v>
-      </c>
+        <v>44146</v>
+      </c>
+      <c r="AM123" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="124" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AL124" s="3"/>
+    </row>
+    <row r="125" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AL125" s="3"/>
+    </row>
+    <row r="126" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AL126" s="3"/>
+    </row>
+    <row r="127" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AL127" s="3"/>
+    </row>
+    <row r="128" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AL128" s="3"/>
+    </row>
+    <row r="129" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL129" s="3"/>
+    </row>
+    <row r="130" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL130" s="3"/>
+    </row>
+    <row r="131" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL131" s="3"/>
+    </row>
+    <row r="132" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL132" s="3"/>
+    </row>
+    <row r="133" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL133" s="3"/>
+    </row>
+    <row r="134" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL134" s="3"/>
+    </row>
+    <row r="135" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL135" s="3"/>
+    </row>
+    <row r="136" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL136" s="3"/>
+    </row>
+    <row r="137" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL137" s="3"/>
+    </row>
+    <row r="138" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL138" s="3"/>
+    </row>
+    <row r="139" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL139" s="3"/>
+    </row>
+    <row r="140" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL140" s="3"/>
+    </row>
+    <row r="141" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL141" s="3"/>
+    </row>
+    <row r="142" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL142" s="3"/>
+    </row>
+    <row r="143" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL143" s="3"/>
+    </row>
+    <row r="144" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL144" s="3"/>
+    </row>
+    <row r="145" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL145" s="3"/>
+    </row>
+    <row r="146" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL146" s="3"/>
+    </row>
+    <row r="147" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL147" s="3"/>
+    </row>
+    <row r="148" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL148" s="3"/>
+    </row>
+    <row r="149" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL149" s="3"/>
+    </row>
+    <row r="150" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL150" s="3"/>
+    </row>
+    <row r="151" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL151" s="3"/>
+    </row>
+    <row r="152" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL152" s="3"/>
+    </row>
+    <row r="153" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL153" s="3"/>
+    </row>
+    <row r="154" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL154" s="3"/>
+    </row>
+    <row r="155" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL155" s="3"/>
+    </row>
+    <row r="156" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL156" s="3"/>
+    </row>
+    <row r="157" spans="38:38" x14ac:dyDescent="0.35">
+      <c r="AL157" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>